<commit_message>
Decimal.TryParse(), int.TryParse() is added.
</commit_message>
<xml_diff>
--- a/Other/CodeComments.xlsx
+++ b/Other/CodeComments.xlsx
@@ -166,7 +166,7 @@
 Ну и путь к файлу/папке надо проверять на существование. И например если не существует - создать / выбросить ошибку.</t>
   </si>
   <si>
-    <t>Прихуярил асинхронные методы, но чето не нравится мне Task(...).Result</t>
+    <t>Прихуяриль параллельный парсинг по каждому сайту. Хз это ли имелось ввиду. Асинхронно вызывать GetHtmlDocumentFromWeb смысла особого нет, так как сразу же используется результат данного метода. Один хуй ждать придется</t>
   </si>
 </sst>
 </file>
@@ -213,7 +213,13 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -249,47 +255,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -312,8 +277,8 @@
       <calculatedColumnFormula>ROW(B2)-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Вып."/>
-    <tableColumn id="4" name="Замечание" dataDxfId="10"/>
-    <tableColumn id="5" name="Примечание" dataDxfId="9"/>
+    <tableColumn id="4" name="Замечание" dataDxfId="1"/>
+    <tableColumn id="5" name="Примечание" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -584,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +559,7 @@
     <col min="2" max="2" width="3.85546875" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="90.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="55.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -866,13 +831,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>2</v>
@@ -948,23 +913,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E25">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$C1=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$C1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:D1048576">
-    <cfRule type="expression" dxfId="2" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>#REF!=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:E25">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$C2=3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
All comments fixed. GettinHtmlAsync is realized.
</commit_message>
<xml_diff>
--- a/Other/CodeComments.xlsx
+++ b/Other/CodeComments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20250" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
   <si>
     <t>Вместо "\n" используй Environment.NewLine</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Столбец1</t>
   </si>
   <si>
-    <t>Пока не понятно должно быть видно за пределами</t>
-  </si>
-  <si>
     <t>Alpha3Code - код валюты из трех букв</t>
   </si>
   <si>
@@ -168,12 +165,65 @@
   <si>
     <t>Прихуяриль параллельный парсинг по каждому сайту. Хз это ли имелось ввиду. Асинхронно вызывать GetHtmlDocumentFromWeb смысла особого нет, так как сразу же используется результат данного метода. Один хуй ждать придется</t>
   </si>
+  <si>
+    <t>А первое значение в enum должно быть None - неопределенность. Enum на самом деле это int (если не унаследуешь от другого типа). А у числа значение по умолчанию 0. 
+Поэтому если какой-то погромист забудет его заполнить, то можно оказаться в заблуждении, если вместо None будет какое-то смысловое. 
+Либо присваивать значениям enum'a явные коды, типа Succes = 1, Error = 2</t>
+  </si>
+  <si>
+    <t>Ебнуть пивка в среду</t>
+  </si>
+  <si>
+    <t>Явно Dispose() вызывать не нужно. Заверни stream в using  
+&gt;WriteToFile
+Если метод асинхронный, его название должно заканчиваться на Async  
+&gt;async void
+Опасное сочетание. В таком случае вызывающий код не дождется выполнения. Поменяй на async Task. 
+рекомендую статью
+https://habr.com/ru/post/452094/</t>
+  </si>
+  <si>
+    <t>Почитать статью</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currencyDataList
+Создаешь рано. Если условие if (htmlDocument != null) не выполнится, то только зря выделил память. 
+</t>
+  </si>
+  <si>
+    <t>// Результат запроса к банку.
+// Получить html страницу.
+// Хранилище данных валюты.
+Подробные комментарии внутри метода не нужны. Что делает код должно быть понятно просто читая его как книгу. Поэтому важно давать длинные, исчерпывающие названия классам, полям и методам. А комментировать в методе надо только не очевидные вещи.</t>
+  </si>
+  <si>
+    <t>Следить за комментариями в процессе разработки</t>
+  </si>
+  <si>
+    <t>var banks = Task.WhenAll(tasks).Result;
+Так тоже не делают. Поменяй на
+var banks = await Task.WhenAll(tasks);</t>
+  </si>
+  <si>
+    <t>Конструкция (…).Result поднялась в метод Program, который асинхронным в текущей версии студии/языка сделать нельзя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thread.Sleep(sleep);
+Это блокирующая операция. В асинхронных методах используй await Task.Delay(sleep); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">await Task.Run(() =&gt; ......
+От этого поизбавляйся везде. Такое можно делать только когда синхронный метод никак нельзя сделать асинхронным </t>
+  </si>
+  <si>
+    <t>Пока не понятно что должно быть видно за пределами</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +231,13 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,17 +260,143 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -238,6 +421,34 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -269,16 +480,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:E25" totalsRowShown="0">
-  <autoFilter ref="A1:E25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:E33" totalsRowShown="0">
+  <autoFilter ref="A1:E33"/>
   <tableColumns count="5">
     <tableColumn id="6" name="Столбец1"/>
     <tableColumn id="1" name="№">
       <calculatedColumnFormula>ROW(B2)-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Вып."/>
-    <tableColumn id="4" name="Замечание" dataDxfId="1"/>
-    <tableColumn id="5" name="Примечание" dataDxfId="0"/>
+    <tableColumn id="4" name="Замечание" dataDxfId="18"/>
+    <tableColumn id="5" name="Примечание" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -547,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +845,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -646,7 +857,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -687,7 +898,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -696,13 +907,13 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -730,7 +941,7 @@
         <v>19</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -787,10 +998,10 @@
         <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -803,7 +1014,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -812,11 +1023,11 @@
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -828,10 +1039,10 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -843,10 +1054,10 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -855,11 +1066,11 @@
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -872,7 +1083,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -885,56 +1096,178 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>43801</v>
+      </c>
+      <c r="B26">
+        <f>ROW(B26)-1</f>
+        <v>25</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f>ROW(B27)-1</f>
+        <v>26</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f>ROW(B28)-1</f>
+        <v>27</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f>ROW(B29)-1</f>
+        <v>28</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <f>ROW(B30)-1</f>
+        <v>29</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f>ROW(B31)-1</f>
+        <v>30</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <f>ROW(B32)-1</f>
         <v>31</v>
       </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="2:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="1"/>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <f>ROW(B33)-1</f>
+        <v>32</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:E25">
-    <cfRule type="expression" dxfId="6" priority="2">
+  <conditionalFormatting sqref="A1:E33">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$C1=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$C1=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A26:D1048576">
-    <cfRule type="expression" dxfId="4" priority="8">
+  <conditionalFormatting sqref="A26:D28 A37:D1048576 A29:C36">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>#REF!=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:E25">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="A2:E33">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$C2=3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Mapster IDictionary <string, string[]> issue
</commit_message>
<xml_diff>
--- a/Other/CodeComments.xlsx
+++ b/Other/CodeComments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Вместо "\n" используй Environment.NewLine</t>
   </si>
@@ -217,6 +217,92 @@
   </si>
   <si>
     <t>Пока не понятно что должно быть видно за пределами</t>
+  </si>
+  <si>
+    <t>В классе Program не должно быть бизнес-логики. Это точка входа в программу, здесь д.б. только метод Main. Все остальные методы надо вынести в сервисы.</t>
+  </si>
+  <si>
+    <t>&gt;GetBankRatesAsync(requests).Result;
+await GetBankRatesAsync(requests);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;var requestsFileName = @"D:\Projects\RatesParsing\RatesParsingConsole\RatesParsingConsole\Scripts\Requests.json";
+var requestsFileName = Path.Combine(Directory.GetCurrentDirectory(), @"\Scripts\Requests.json"); </t>
+  </si>
+  <si>
+    <t>&gt;WriteToFileAsync(banks);
+await WriteToFileAsync(banks);</t>
+  </si>
+  <si>
+    <t>&gt;if (requestType == GetRequestType.FromCode)
+Для обработки значений enum используй switch</t>
+  </si>
+  <si>
+    <t>&gt;var tasks = new List&lt;Task&lt;BankRatesModel»();
+var tasks = new List&lt;Task&lt;BankRatesModel»(requests.Count());</t>
+  </si>
+  <si>
+    <t>&gt;GetBankRequestsFromCode
+Названия локальных переменных д.б. с маленькой буквы</t>
+  </si>
+  <si>
+    <t>&gt;{"GetNumberFromText", new string[0]}
+Вместо new string[0] используй
+Array.Empty&lt;string&gt;()</t>
+  </si>
+  <si>
+    <t>&gt;BankRequestDto
+В моделях старайся использовать интерфейсы, а не явные реализации. Так код становится более гибким.
+Вместо
+public Dictionary&lt;string, string[]&gt; UnitScripts { get; set; }
+public IDictionary&lt;string, string[]&gt; UnitScripts { get; set; }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;using (StreamReader sr = new StreamReader(fileName, System.Text.Encoding.UTF8))
+&gt;JsonText = sr.ReadToEnd();
+Можно сделать асинхронным.
+Или вообще написать в 1 строчку:
+jsonText = await File.ReadAllTextAsync(fileName, System.Text.Encoding.UTF8); </t>
+  </si>
+  <si>
+    <t>&gt;public BankRatesModel GetBankRates(BankRequestDto request)
+закомментировать неиспользуемое</t>
+  </si>
+  <si>
+    <t>&gt;List&lt;CurrencyDataModel&gt; currencyDataList;
+Все равно рано создаешь объект. Он же не нужен за пределами блока if.</t>
+  </si>
+  <si>
+    <t>&gt;ProcessingResultModel.ProcessingResult.Success
+Можно убрать "ProcessingResultModel."</t>
+  </si>
+  <si>
+    <t>В BankRatesModel можно сделать метод
+public void SetErrorResponse(string message)
+{
+RequestResultStatus = ProcessingResult.Error;
+RequestResultMessage = message;
+ExchangeRates = Array.Empty&lt;CurrencyDataModel&gt;();
+}
+А потом просто вызвать
+bankRates.SetErrorResponse("Ошибка при получении html страницы.");
+Скрываем детали, и меньше кода писать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кстати постфикс Model только для выходных моделей, которые видит юзер/метод публичного интерфейса
+Для доменных (которые положишь в хранилище) постфиксы не нужны </t>
+  </si>
+  <si>
+    <t>Да, но есть клевые инструменты для автомапинг. Ставь либу Mapster</t>
+  </si>
+  <si>
+    <t>Применена конструкция .Result, так как применение await требует соответственно сделать входной метод Program.Main(), что недопустимо в текущей версии языка.</t>
+  </si>
+  <si>
+    <t>Оказывается надо подключить LINQ чтобы отобразился метод расширения Count()</t>
+  </si>
+  <si>
+    <t>mapster выебуется. Оставил как есть. Разобраться надо</t>
   </si>
 </sst>
 </file>
@@ -260,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -268,16 +354,19 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -313,159 +402,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -480,16 +416,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:E33" totalsRowShown="0">
-  <autoFilter ref="A1:E33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:E49" totalsRowShown="0">
+  <autoFilter ref="A1:E49"/>
   <tableColumns count="5">
     <tableColumn id="6" name="Столбец1"/>
     <tableColumn id="1" name="№">
       <calculatedColumnFormula>ROW(B2)-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Вып."/>
-    <tableColumn id="4" name="Замечание" dataDxfId="18"/>
-    <tableColumn id="5" name="Примечание" dataDxfId="17"/>
+    <tableColumn id="4" name="Замечание" dataDxfId="1"/>
+    <tableColumn id="5" name="Примечание" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -758,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,7 +1063,7 @@
         <v>43801</v>
       </c>
       <c r="B26">
-        <f>ROW(B26)-1</f>
+        <f t="shared" ref="B26:B33" si="1">ROW(B26)-1</f>
         <v>25</v>
       </c>
       <c r="C26" s="1">
@@ -1140,7 +1076,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27">
-        <f>ROW(B27)-1</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C27" s="1">
@@ -1153,7 +1089,7 @@
     </row>
     <row r="28" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="B28">
-        <f>ROW(B28)-1</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C28" s="1">
@@ -1168,26 +1104,26 @@
     </row>
     <row r="29" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="B29">
-        <f>ROW(B29)-1</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" ht="77.25" x14ac:dyDescent="0.25">
       <c r="B30">
-        <f>ROW(B30)-1</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1196,73 +1132,281 @@
     </row>
     <row r="31" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B31">
-        <f>ROW(B31)-1</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>44</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="B32">
-        <f>ROW(B32)-1</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B33">
-        <f>ROW(B33)-1</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D36" s="4"/>
+    <row r="34" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>43805</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ref="B34:B49" si="2">ROW(B34)-1</f>
+        <v>33</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="C43" s="1">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="C44" s="1">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="C45" s="1">
+        <v>3</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="C46" s="1">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="C47" s="1">
+        <v>3</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E49" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:E33">
-    <cfRule type="expression" dxfId="4" priority="2">
+  <conditionalFormatting sqref="A1:E49">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$C1=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$C1=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A26:D28 A37:D1048576 A29:C36">
-    <cfRule type="expression" dxfId="2" priority="8">
+  <conditionalFormatting sqref="A26:D28 A37:D48 A29:C36 C35:C48 A50:D1048576 A49:C49">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>#REF!=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:E33">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A2:E49">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$C2=3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add serialization of exchange rates in .json file.
</commit_message>
<xml_diff>
--- a/Other/CodeComments.xlsx
+++ b/Other/CodeComments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RatesParsing\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\WEB\ASP\RatesParsing\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
   <si>
     <t>Вместо "\n" используй Environment.NewLine</t>
   </si>
@@ -303,6 +303,138 @@
   </si>
   <si>
     <t>mapster выебуется. Оставил как есть. Разобраться надо</t>
+  </si>
+  <si>
+    <t>1. При конфигурации строковых полей, обозначь им максимально возможную длину (HasMaxLength). MAX это 2 ГБ, такое вряд ли где-то нужно. Например код валюты всегда 3, Url не может быть длиннее 2000 символов. А вот длину скрипта лучше не ограничивать.</t>
+  </si>
+  <si>
+    <t>6. CurrencySerializer это сервис. Значит он не должен никогда возвращать доменные модели. Пускай метод GetCurrenciesFromXml возвращает IEnumerable&lt;CurrencyXmlItem&gt;, а маппинг в доменную делай непосредственно там где сохраняешь.</t>
+  </si>
+  <si>
+    <t>2. modelBuilder.Entity&lt;ExchangeRateList&gt;().Property(i =&gt; i.DateTimeStamp).IsRequired();
+DateTime это структура - значимый тип. Т.е. она IsRequired() по умолчанию, если ты явно не сделаешь её nullable.</t>
+  </si>
+  <si>
+    <t>3. foreach(var curr in currencies)
+{
+context.Currencies.Add(curr);
+}
+Можно заменить одной строкой:
+context.Currencies.AddRange(currencies);</t>
+  </si>
+  <si>
+    <t>4. string fileName = string.Concat(workingDirectory, xmlRelativeFilePath);
+Используй Path.Combine()</t>
+  </si>
+  <si>
+    <t>5. var currencies = new List&lt;Currency&gt;();
+var currencies = new List&lt;Currency&gt;(currenciesFromXmlNoDuplicates.Count());</t>
+  </si>
+  <si>
+    <t>7. Теперь архитектурно. С BankRatesContext должен работать один единственный класс, и никто больше про его существование знать не должен.
+Схема такая:
+1) Делаешь класс RepositoryBase&lt;T&gt; в котором реализуешь все необходимые тебе методы для работы с сущностями БД (CRUD + может что-то еще).
+2) Делаешь интерфейс IRepository&lt;T&gt; в котором эти методы объявляешь.
+3) Для каждой доменной сущности должен быть свой интерфейс и реализация репозитория:
+IBankRepository : IRepository&lt;Bank&gt;
+BankRepository : RepositoryBase&lt;Bank&gt;, IBankRepository
+Т.е. работать с доменными сущностями ты должен всегда только через соотв. ему интерфейс репозитория.
+Получать объекты репозиториев/сервисов надо с помощью Dependency Injection.</t>
+  </si>
+  <si>
+    <t>1. В объявление RepositoryBase&lt;T&gt; и IRepository&lt;T&gt; добавь ограничение на тип параметра
+where T : class
+Чтобы в &lt;T&gt; нельзя было засунуть какую-нибудь хуйню вроде int или struct.</t>
+  </si>
+  <si>
+    <t>2. Неправильно сделан асинхронный метод.
+public void AddAndSaveAsync(T t)
+{
+context.Add(t);
+context.SaveChangesAsync();
+}
+Должно быть так:
+public async Task AddAndSaveAsync(T t)
+{
+await context.AddAsync(t);
+await context.SaveChangesAsync();
+}
+Пока можешь просто запомнить синтаксис. Но потом изучи статьи про таски и асинхронное программирование в .NET, этот пробел надо заполнить.</t>
+  </si>
+  <si>
+    <t>3. Реализуй больше методов в RepositoryBase.
+public interface IRepository&lt;T&gt; where T : class
+{
+Task AddAsync(T entity);
+Task AddRangeAsync(T[] entity);
+Task&lt;T&gt; GetByIdAsync(int id);
+Task&lt;T&gt; GetFirstOrDefaultAsync(Expression&lt;Func&lt;T, bool» where);
+Task&lt;IEnumerable&lt;T» GetAllAsync();
+Task&lt;IEnumerable&lt;T» GetManyAsync(Expression&lt;Func&lt;T, bool» where);
+Task&lt;bool&gt; AnyAsync(Expression&lt;Func&lt;T, bool» where);
+Task&lt;int&gt; CountAsync(Expression&lt;Func&lt;T, bool» where = null);
+IQueryable&lt;T&gt; Query();
+Task CommitAsync();
+}
+В итоге, в других репозиториях в 99% случаев не надо будет писать какие-то дополнительные методы, поскольку базовые, из списка выше, покрывают практически все операции которые могут понадобится при работе с БД.</t>
+  </si>
+  <si>
+    <t>4. Не нравится как заполняешь БД данными. Хорошо конечно что разобрался с десериализацией XML, может пригодится. Но так не делается. Накатывать все надо миграциями. Миграции, помимо удобного инструмента развертывания и обновления БД, выполняют функцию версионирования. Т.е. читая их, можно увидеть все что происходило с базой за время жизни приложения. И другими способами в базе что-то изменять нельзя - это стандарт и best practice.
+Можно воспользоваться методом HasData:
+modelBuilder.Entity&lt;Bank&gt;().HasData(new Bank { BankName = "Bank1" }, new Bank { BankName = "Bank2" });
+Или создать новую миграцию со скриптом:
+migrationBuilder.Sql("INSERT INTO Banks VALUES ( (...), (...) );</t>
+  </si>
+  <si>
+    <t>Разобраться со скриптом</t>
+  </si>
+  <si>
+    <t>1. IBankRepository -&gt; IEnumerable&lt;Currency&gt; GetCurrencies();
+Репозиторий работает только со своей доменной моделью. Для курсов создай ICurrencyRepository и т.д.</t>
+  </si>
+  <si>
+    <t>2. ToListAsync(), ToList().
+Если метод возвращает IEnumerable&lt;T&gt;, то лучше приводи коллекцию к массиву. Воспользоваться коллекцией как List-ом с вызывающей стороны все-равно будет нельзя, а массив 1) создается быстрее чем динамический список; 2) потребляем меньше памяти.</t>
+  </si>
+  <si>
+    <t>3. AsNoTracking()
+А если я хочу получить все банки и что-то изменить в них? Не используй AsNoTracking() в методах общего назначения.</t>
+  </si>
+  <si>
+    <t>4. В классе RepositoryBase сделай все методы как vitual. Сейчас только GetAll().</t>
+  </si>
+  <si>
+    <t>5. public async Task AddRangeAsync(T[] entity) =&gt; await _context.AddRangeAsync(entity);
+Поскольку метод больше нихера не делает, кроме того что пробрасывает вызов другого асинхронного метода, можно избавиться от async/await. Тем самым мы немного увеличим производительность, за счет того что CLR будет создано меньше на одну машину состояний.
+public Task AddRangeAsync(T[] entity) =&gt; _context.AddRangeAsync(entity);</t>
+  </si>
+  <si>
+    <t>6. @Html.DisplayNameFor(model =&gt; model.Banks.First().Name)
+А если коллекция не инициализирована или не содержит элементов? Страница упадет с исключением.
+Когда уже проверил коллекцию на null и Any(), и все-таки хочешь первый элемент, не вычисляй его каждый раз. Вынеси model.Banks.First() в объект и обращайся дальше к нему.</t>
+  </si>
+  <si>
+    <t>7. private readonly IBankRepository _context;
+Название обманывает.
+Если сотрёшь " _context;" и нажмешь пробел, студия предложит тебе название объекта по best practice.
+Получится: private readonly IBankRepository bankRepository;</t>
+  </si>
+  <si>
+    <t>8. OnGetAsync(int? id)
+Зачем вообще допускать null value в id? Логично же, что если мы хотим отредактировать элемент, идентификатор элемента обязателен.</t>
+  </si>
+  <si>
+    <t>9. BankDomain = await _context.GetByIdAsync(id);
+А вот сразу после этой строки надо проверить BankDomain на null, т.к. метод FindAsync() может его вернуть если ничего не найдет в БД.
+Короче перенести выше BankExists(), а от блока try/catch вообще избавиться, их не должно быть на уровне контроллера. С EF у тебя работает слой Storage, ни про какие DbUpdateConcurrencyException класс EditModel знать не должен.</t>
+  </si>
+  <si>
+    <t>10. domain.Currency = _context.GetCurrencies().FirstOrDefault(i =&gt; i.Id == model.Id);
+Можно просто поменять CurrencyId и избежать запроса к базе.
+Ну и используй лучше Mapster в случае такого простого маппинга. Только названия полей приведи к одинаковому виду (CurrencyID &gt; CurrencyId).</t>
+  </si>
+  <si>
+    <t>Пока забил хуй</t>
   </si>
 </sst>
 </file>
@@ -346,13 +478,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -360,47 +491,260 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="38">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -416,16 +760,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:E49" totalsRowShown="0">
-  <autoFilter ref="A1:E49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:E70" totalsRowShown="0">
+  <autoFilter ref="A1:E70"/>
   <tableColumns count="5">
-    <tableColumn id="6" name="Столбец1"/>
+    <tableColumn id="6" name="Столбец1" dataDxfId="0"/>
     <tableColumn id="1" name="№">
       <calculatedColumnFormula>ROW(B2)-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Вып."/>
-    <tableColumn id="4" name="Замечание" dataDxfId="1"/>
-    <tableColumn id="5" name="Примечание" dataDxfId="0"/>
+    <tableColumn id="4" name="Замечание" dataDxfId="37"/>
+    <tableColumn id="5" name="Примечание" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -694,19 +1038,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="90.7109375" customWidth="1"/>
-    <col min="5" max="5" width="55.85546875" customWidth="1"/>
+    <col min="4" max="4" width="118" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -726,7 +1070,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43793</v>
       </c>
@@ -742,7 +1086,8 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
       <c r="B3">
         <f t="shared" ref="B3:B25" si="0">ROW(B3)-1</f>
         <v>2</v>
@@ -756,6 +1101,7 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
       <c r="B4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -769,6 +1115,7 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
       <c r="B5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -782,6 +1129,7 @@
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
       <c r="B6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -797,6 +1145,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
       <c r="B7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -810,6 +1159,7 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
       <c r="B8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -823,6 +1173,7 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
       <c r="B9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -838,6 +1189,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
       <c r="B10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -853,6 +1205,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
       <c r="B11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -866,6 +1219,7 @@
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
       <c r="B12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -881,6 +1235,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
       <c r="B13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -893,7 +1248,8 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
       <c r="B14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -907,6 +1263,7 @@
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
       <c r="B15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -938,6 +1295,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
       <c r="B17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -950,7 +1308,8 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
       <c r="B18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -963,7 +1322,8 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
       <c r="B19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -978,7 +1338,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
       <c r="B20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -994,6 +1355,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
       <c r="B21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1007,6 +1369,7 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
       <c r="B22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1019,7 +1382,8 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
       <c r="B23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1033,6 +1397,7 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
       <c r="B24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1045,7 +1410,8 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
       <c r="B25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1059,7 +1425,7 @@
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>43801</v>
       </c>
       <c r="B26">
@@ -1075,6 +1441,7 @@
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
       <c r="B27">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1087,7 +1454,8 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
       <c r="B28">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1102,7 +1470,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
       <c r="B29">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1110,12 +1479,13 @@
       <c r="C29" s="1">
         <v>1</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
       <c r="B30">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -1123,7 +1493,7 @@
       <c r="C30" s="1">
         <v>1</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1131,6 +1501,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
       <c r="B31">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -1138,12 +1509,13 @@
       <c r="C31" s="1">
         <v>1</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
       <c r="B32">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -1151,12 +1523,13 @@
       <c r="C32" s="1">
         <v>1</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
       <c r="B33">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -1164,7 +1537,7 @@
       <c r="C33" s="1">
         <v>1</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E33" s="1" t="s">
@@ -1182,12 +1555,13 @@
       <c r="C34" s="1">
         <v>1</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
       <c r="B35">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -1195,12 +1569,13 @@
       <c r="C35" s="1">
         <v>1</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
       <c r="B36">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -1208,12 +1583,13 @@
       <c r="C36" s="1">
         <v>1</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
       <c r="B37">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -1229,6 +1605,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
       <c r="B38">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -1241,7 +1618,8 @@
       </c>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
       <c r="B39">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -1257,6 +1635,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
       <c r="B40">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -1270,6 +1649,7 @@
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
       <c r="B41">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -1282,7 +1662,8 @@
       </c>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
       <c r="B42">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -1298,6 +1679,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
       <c r="B43">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -1308,9 +1690,12 @@
       <c r="D43" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
       <c r="B44">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -1321,9 +1706,12 @@
       <c r="D44" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="1"/>
+      <c r="E44" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
       <c r="B45">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -1334,9 +1722,12 @@
       <c r="D45" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
       <c r="B46">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -1347,9 +1738,12 @@
       <c r="D46" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E46" s="1"/>
+      <c r="E46" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
       <c r="B47">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -1360,9 +1754,12 @@
       <c r="D47" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="E47" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
       <c r="B48">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -1375,7 +1772,8 @@
       </c>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
       <c r="B49">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -1383,30 +1781,305 @@
       <c r="C49" s="1">
         <v>1</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E49" s="1"/>
     </row>
+    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>43847</v>
+      </c>
+      <c r="B50">
+        <f>ROW(B50)-1</f>
+        <v>49</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51">
+        <f t="shared" ref="B51:B52" si="3">ROW(B51)-1</f>
+        <v>50</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53">
+        <f t="shared" ref="B53:B60" si="4">ROW(B53)-1</f>
+        <v>52</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>43848</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="4"/>
+        <v>56</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58">
+        <f t="shared" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59">
+        <f t="shared" si="4"/>
+        <v>58</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+      <c r="C60" s="1">
+        <v>2</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>43851</v>
+      </c>
+      <c r="B61">
+        <f>ROW(B61)-1</f>
+        <v>60</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62">
+        <f>ROW(B62)-1</f>
+        <v>61</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63">
+        <f>ROW(B63)-1</f>
+        <v>62</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64">
+        <f>ROW(B64)-1</f>
+        <v>63</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65">
+        <f>ROW(B65)-1</f>
+        <v>64</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66">
+        <f>ROW(B66)-1</f>
+        <v>65</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67">
+        <f>ROW(B67)-1</f>
+        <v>66</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68">
+        <f>ROW(B68)-1</f>
+        <v>67</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69">
+        <f>ROW(B69)-1</f>
+        <v>68</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="B70">
+        <f>ROW(B70)-1</f>
+        <v>69</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E70" s="1"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:E49">
-    <cfRule type="expression" dxfId="6" priority="2">
+  <conditionalFormatting sqref="A1:E70">
+    <cfRule type="expression" dxfId="32" priority="2">
       <formula>$C1=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="31" priority="3">
       <formula>$C1=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A26:D28 A37:D48 A29:C36 C35:C48 A50:D1048576 A49:C49">
-    <cfRule type="expression" dxfId="4" priority="8">
+  <conditionalFormatting sqref="A26:D28 A29:C36 A37:D1048576 C35:C56">
+    <cfRule type="expression" dxfId="30" priority="8">
       <formula>#REF!=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:E49">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="A2:E70">
+    <cfRule type="expression" dxfId="28" priority="1">
       <formula>$C2=3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>